<commit_message>
Add tab to test prompts against the dataset
</commit_message>
<xml_diff>
--- a/important-files/email-2-quote-dataset.xlsx
+++ b/important-files/email-2-quote-dataset.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juliusz.gorzen\PycharmProjects\email-to-quote-streamlit\important-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juliusz.gorzen\Desktop\email-2-quote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42034144-577E-4411-AB00-32DFEBD142A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44D95F5-5431-46FA-AD96-C3A4E257F005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mails" sheetId="1" r:id="rId1"/>
     <sheet name="objects" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mails!$A$1:$I$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mails!$A$1:$J$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">objects!$A$1:$H$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="344">
   <si>
     <t>Hej, Musimy dostarczyć część naszego SKU 12345 z Krakowa do Katowic. Odbiór zaplanowano na 5 kwietnia 2024 r. Będzie to 12 palet z 14 tonami produktów. Będą dwa miejsca odbioru, oba w Krakowie. Cała reszta w standardzie. Czekam na wycenę. To, co najlepsze</t>
   </si>
@@ -1144,24 +1144,6 @@
   </si>
   <si>
     <t>{
-  "conversationId": "gWuIPOjl3ke4r4gx6GOEV5UFu6q46pmQYwsID7vo7UpABLq51C6yVYtqT8BxrmL7Oq27on3YI8nDomEl",
-  "body": "Buna ziua ,\n \nPermiteti-mi sa revin la solicitarea de oferta  pret pentru un transport despre care am discutat anul trecut .\n“Rog oferta dumneavoastra de pret pentru un transport de 17,00 TO  marfa amablaj ( folii de plastic care folosim ptr impachetarea sacilor de ingrasaminte de 50 kg. ) pentru ruta depozit Fratesti/Giurgiu la  HU- 3580 Tiszaujváros .\nTransportul nu este un camion complet de 24 TO”\n",
-  "sender": {
-    "emailAddress": "di53a@jualcloud.net",
-    "displayName": ""
-  },
-  "recipient": [
-    {
-      "emailAddress": "contactjosegaytan@elinore1818.site",
-      "displayName": ""
-    }
-  ],
-  "date": "2024-02-24T16:11:32.511Z",
-  "subject": ""
-}</t>
-  </si>
-  <si>
-    <t>{
   "conversationId": "sVshL9XmnoQFPbQPDN9bu6cAiyXnL9t6Y7W0w6hydN1F7P48Vr471M4PlUxAkMU1Mec7vGS7kHf3835f",
   "body": "Buna ziua\nVa rog ma ajutati cu o cotatie  de pret  pentru un transport din TURCIA:\n \nUn palet tabla inox-1035 kg\n \nexp:\nLoading Address:\nTeknik Metal A.S.\nOsmangazi Mah. 3143 sok. No: 7 Esenyurt Istanbul Turkey 34522\nContact person: Serdar Yeşilkaya\n+90 212 665 0404\n \nGoogle maps:\nhttps://goo.gl/maps/CuuqUxkJGXz\n\n\n\n\ndest:\nSC KOBER SRL SUCURSALA VADURI Com Alexandru  Cel Bun,  CP 617511 str ZORELELOR 25 LOCALITATE VADURI, JUD NEAMT, ROMANIA\nMultumesc.\n",
   "sender": {
@@ -1197,9 +1179,6 @@
 }</t>
   </si>
   <si>
-    <t>[{"origin_location":"Werk Bobingen, Lindauer Straße 70, 86399 Bobingen","destination_location":"520077 Sfantu Gheorghe, jud. Covasna","currency":"EUR","distance":0,"transport_type":"FTL","trailer_type":"13.6 curtain trailer","dangerous_hazardous":"No","cargo_type":"General","steps":[],"validity_date":"","loading_date":"2024-02-05T00:00:00Z","arrival_date":"","weight":11000,"volume":0,"pallets":[],"vehicle_loading_method":"vehicle rear loading","temperature_requirements":[],"seals":false}]</t>
-  </si>
-  <si>
     <t>[{"origin_location":"300283 Timisoara, Romania","destination_location":"4715-405 Braga, Portugal","currency":"EUR","distance":0,"transport_type":"FTL","trailer_type":"13.6 curtain trailer","dangerous_hazardous":"No","cargo_type":"General","steps":[],"validity_date":"","loading_date":"","arrival_date":"","weight":155,"volume":0,"pallets":[{"amount":1,"type":"pallet 800x1200"}],"vehicle_loading_method":"vehicle rear loading","temperature_requirements":[],"seals":false}]</t>
   </si>
   <si>
@@ -1242,24 +1221,6 @@
 }</t>
   </si>
   <si>
-    <t>{
-  "conversationId": "QzHeJ8GUFLAX1rV89F6M5lxCyG11lSGvoqyxuQhGVlFX4X0Ecv3r0bdTo64LQy4cBiaw4TxCSqGq2elA",
-  "body": "Hello.\nIs it possible to pick up some pallets from Blästerteknik Gislaved to morrow? And deliver it to Sibbhult tomorrow or Monday?",
-  "sender": {
-    "emailAddress": "fjiohio@estudiosucre.com",
-    "displayName": ""
-  },
-  "recipient": [
-    {
-      "emailAddress": "klimenkovmaksim@filevino.com",
-      "displayName": ""
-    }
-  ],
-  "date": "2024-03-14T06:34:11.110Z",
-  "subject": "Pallets from Blästerteknik Gislaved to Sibbhult",
-}</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -1359,24 +1320,6 @@
   ],
   "date": "2024-03-18T07:53:56.103Z",
   "subject": ""
-}</t>
-  </si>
-  <si>
-    <t>{
-  "conversationId": "29v8t0ALv4z0os8R8G97A92JnueL23mRzTv9VN6Q72I4y9eTiWb0qCshrp4UxQ6U50tff0vmtZw8r13r",
-  "body": "We received RFQ from our automotive customer for below two lines:\nFR-59000 to GB - OX16 4TG, Single trip, Mega trailer, 20 trailers per week.\nGB - OX16 4TG to FR-42230, Single trip, Mega trailer, 15 trailers per week.\n\n Additional details below:\n·         Automotive Customer.\n·         Goods - Automotive Components.\n·         A just-in-time environment.\n·         95% of GPS requirement.\n·         Customs clearance should be on collection sites.\n·         Minimum notification 24h before collection.\n\n Deadline for this RFQ is 26/02/2024.",
-  "sender": {
-    "emailAddress": "mark_smith-cargo@domain.com",
-    "displayName": "Mark Smith"
-  },
-  "recipient": [
-    {
-      "emailAddress": "cardansgiro@evgeniyvis.com",
-      "displayName": ""
-    }
-  ],
-  "date": "2024-02-11T13:41:06.006Z",
-  "subject": "Transportation RFQ from Automotive Customer",
 }</t>
   </si>
   <si>
@@ -1417,24 +1360,6 @@
 Are the Goods controlled (require license/additional customs checks)? No
 Have you shipped before? Yes
 Product type: Toiletries, household cleaning products</t>
-  </si>
-  <si>
-    <t>{
-  "conversationId": "9jGfNk68eG0h2Wjlj8wAOdXeNxl36ZtqLGzrFBiC2F6hQ2XIA2Y5TIIb7d3Mz5Dpg1b47TyWZV6Srd5N",
-  "body": "2 FTL’s , non haz. Goods are wholesale dry goods.\nStandard curtainsided tautliner is fine\nCollection\nUnit 6, Elm Farm Ind. Estate, Edison Road, Bedford, Bedfordshire MK41 0HR\nDelivery\nCP  30870 Mazarrón\nMurcia - España\n \nFor the customs team:\nIncoterms\nDAP\nAverage number of HS codes (commodity codes) per shipment\n1-3\nOrigin of Goods\nUK\nAre the Goods controlled (require license/additional customs checks)?\nNo\nHave you shipped before\nYes\nProduct type\nToiletries, household cleaning products",
-  "sender": {
-    "emailAddress": "dolds2735@newbreedapps.com",
-    "displayName": ""
-  },
-  "recipient": [
-    {
-      "emailAddress": "keno87@trantienclone.top",
-      "displayName": "Ken"
-    }
-  ],
-  "date": "2024-02-15T15:41:19.541Z",
-  "subject": "New Shipment Request",
-}</t>
   </si>
   <si>
     <t>{
@@ -2478,9 +2403,6 @@
     <t>{"conversationId":"6c1SAK695h43juMAJ2H7x3mF9x637KPWloNnh8JXe8qm0QsQZ3TeCY1l4S85V8cSZ9bJnA0FtrO993jh","body":"Buna,\n \nVa rog sa ne ajuti cu o cotatie de transport pentru 3 paleti - suplimente alimentare, greutate bruta – 458Kg, 120x100x133, luand in considerare urmatoarele:\nExport UK si control sanitar veterinar in Calais, Franta -  in sarcina IB Cargo (DVE + T1);\nControl sanitar veterninar la Calais in sarcina Prisum;\nVama import Otopeni in sarcina Prisum;\nTaxe vamale si TVA in vama la import in sarcina Prisum.\n \nAdresa de incarcare:\nUnit 1 Bridgwater Trade Park.\nA38 Bristol Road,\nBridgwater\nTA6 4WA (or driver can type Easy Bathrooms &amp; Tiles Bridgwater on google maps and our warehouse is near this store)\nProgram depozit: 08.00 – 16.30\nReferinta incarcare: 111681\n","sender":{"emailAddress":"ardentrans@bankcommon.com","displayName":""},"recipient":[{"emailAddress":"misterkiss6@imaanpharmacy.com","displayName":""}],"date":"2024-03-15T14:08:32.432Z","subject":""}</t>
   </si>
   <si>
-    <t>{"conversationId":"gWuIPOjl3ke4r4gx6GOEV5UFu6q46pmQYwsID7vo7UpABLq51C6yVYtqT8BxrmL7Oq27on3YI8nDomEl","body":"Buna ziua ,\n \nPermiteti-mi sa revin la solicitarea de oferta  pret pentru un transport despre care am discutat anul trecut .\n“Rog oferta dumneavoastra de pret pentru un transport de 17,00 TO  marfa amablaj ( folii de plastic care folosim ptr impachetarea sacilor de ingrasaminte de 50 kg. ) pentru ruta depozit Fratesti/Giurgiu la  HU- 3580 Tiszaujváros .\nTransportul nu este un camion complet de 24 TO”\n","sender":{"emailAddress":"di53a@jualcloud.net","displayName":""},"recipient":[{"emailAddress":"contactjosegaytan@elinore1818.site","displayName":""}],"date":"2024-02-24T16:11:32.511Z","subject":""}</t>
-  </si>
-  <si>
     <t>{"conversationId":"sVshL9XmnoQFPbQPDN9bu6cAiyXnL9t6Y7W0w6hydN1F7P48Vr471M4PlUxAkMU1Mec7vGS7kHf3835f","body":"Buna ziua\nVa rog ma ajutati cu o cotatie  de pret  pentru un transport din TURCIA:\n \nUn palet tabla inox-1035 kg\n \nexp:\nLoading Address:\nTeknik Metal A.S.\nOsmangazi Mah. 3143 sok. No: 7 Esenyurt Istanbul Turkey 34522\nContact person: Serdar Yeşilkaya\n+90 212 665 0404\n \nGoogle maps:\nhttps://goo.gl/maps/CuuqUxkJGXz\n\n\n\n\ndest:\nSC KOBER SRL SUCURSALA VADURI Com Alexandru  Cel Bun,  CP 617511 str ZORELELOR 25 LOCALITATE VADURI, JUD NEAMT, ROMANIA\nMultumesc.\n","sender":{"emailAddress":"pde6868@bestmms.cloud","displayName":""},"recipient":[{"emailAddress":"sgtnubbl@pianoxltd.com","displayName":""}],"date":"2024-01-13T06:32:44.043Z","subject":"Transport TURCIA - ROMANIA"}</t>
   </si>
   <si>
@@ -2499,9 +2421,6 @@
     <t>{"conversationId":"w942fOMfy0Cs0mMtxMqQGNal6oY0Q5j1Qu8cNMUziMYTMNOX9T0q2mH7KoZm3Y8Abrh33wrU2UQtVsDR","body":"Goedemorgen Bart,\nWat is jullie tarief voor laden 04.01 in Vreeland 3633 en leveren 09.01 in Falkenberg Zweden\nFTL, lege nieuwe vaten, rond 5-6t\nPallets 274cm hoog!\n","sender":{"emailAddress":"osu2005@hulas.us","displayName":""},"recipient":[{"emailAddress":"appraisers@kreasianakkampoeng.com","displayName":"Bart van der Veen"}],"date":"2024-01-01T15:01:44.000Z","subject":"Vreeland - Falkenberg"}</t>
   </si>
   <si>
-    <t>{ "conversationId": "QzHeJ8GUFLAX1rV89F6M5lxCyG11lSGvoqyxuQhGVlFX4X0Ecv3r0bdTo64LQy4cBiaw4TxCSqGq2elA", "body": "Hello.\nIs it possible to pick up some pallets from Blästerteknik Gislaved to morrow? And deliver it to Sibbhult tomorrow or Monday?", "sender": { "emailAddress": "fjiohio@estudiosucre.com", "displayName": "" }, "recipient": [ { "emailAddress": "klimenkovmaksim@filevino.com", "displayName": "" } ], "date": "2024-03-14T06:34:11.110Z", "subject": "Pallets from Blästerteknik Gislaved to Sibbhult", }</t>
-  </si>
-  <si>
     <t>{"conversationId":"qKNyEudCHKx2j3Nn6F59sG2ZGowjmj8K6bvUO2EHUsOl0So718EDE9W1Tn10Jk2XTx2RIv5KZcR17vk4","body":"Hallo,\nKunnen jullie voor maandag 12/02 een vracht regelen naar onderstaan adres:\nVW Poznan Werk Wrzesnia\nBiałężyce 100\n62-300 Wrzesnia\nLading is 2 dozen 2m*2m*1m\nGewicht is ongeveer 1000kg\nVracht kan afgehaald worden vanaf 8u30\nMet vriendelijke groeten,\nJan","sender":{"emailAddress":"ambrodel@code-gmail.com","displayName":""},"recipient":[{"emailAddress":"almazyan1983@elevecortesias.tech","displayName":""}],"date":"2024-01-09T11:59:11.000Z","subject":"Vracht naar VW Poznan Werk Wrzesnia"}</t>
   </si>
   <si>
@@ -2512,12 +2431,6 @@
   </si>
   <si>
     <t>{"conversationId":"DaUHGu2MBH89ywRJ75aboS8L1R2568ntcXC4DLZzMk99avhdKmtSQ5NG7Zt331W6du3AyvdcJY92uRO8","body":"Can you please price:\nAlfreton – 5667 KX Geldrop NL\nAndover – Nivelles BE\nMany thanks.\n","sender":{"emailAddress":"rmsabo@greenpanel.xyz","displayName":""},"recipient":[{"emailAddress":"ashninartyom@evgeniyvis.website","displayName":""}],"date":"2024-03-18T07:53:56.103Z","subject":""}</t>
-  </si>
-  <si>
-    <t>{ "conversationId": "29v8t0ALv4z0os8R8G97A92JnueL23mRzTv9VN6Q72I4y9eTiWb0qCshrp4UxQ6U50tff0vmtZw8r13r", "body": "We received RFQ from our automotive customer for below two lines:\nFR-59000 to GB - OX16 4TG, Single trip, Mega trailer, 20 trailers per week.\nGB - OX16 4TG to FR-42230, Single trip, Mega trailer, 15 trailers per week.\n\n Additional details below:\n· Automotive Customer.\n· Goods - Automotive Components.\n· A just-in-time environment.\n· 95% of GPS requirement.\n· Customs clearance should be on collection sites.\n· Minimum notification 24h before collection.\n\n Deadline for this RFQ is 26/02/2024.", "sender": { "emailAddress": "mark_smith-cargo@domain.com", "displayName": "Mark Smith" }, "recipient": [ { "emailAddress": "cardansgiro@evgeniyvis.com", "displayName": "" } ], "date": "2024-02-11T13:41:06.006Z", "subject": "Transportation RFQ from Automotive Customer", }</t>
-  </si>
-  <si>
-    <t>{ "conversationId": "9jGfNk68eG0h2Wjlj8wAOdXeNxl36ZtqLGzrFBiC2F6hQ2XIA2Y5TIIb7d3Mz5Dpg1b47TyWZV6Srd5N", "body": "2 FTL’s , non haz. Goods are wholesale dry goods.\nStandard curtainsided tautliner is fine\nCollection\nUnit 6, Elm Farm Ind. Estate, Edison Road, Bedford, Bedfordshire MK41 0HR\nDelivery\nCP 30870 Mazarrón\nMurcia - España\n \nFor the customs team:\nIncoterms\nDAP\nAverage number of HS codes (commodity codes) per shipment\n1-3\nOrigin of Goods\nUK\nAre the Goods controlled (require license/additional customs checks)?\nNo\nHave you shipped before\nYes\nProduct type\nToiletries, household cleaning products", "sender": { "emailAddress": "dolds2735@newbreedapps.com", "displayName": "" }, "recipient": [ { "emailAddress": "keno87@trantienclone.top", "displayName": "Ken" } ], "date": "2024-02-15T15:41:19.541Z", "subject": "New Shipment Request", }</t>
   </si>
   <si>
     <t>{"conversationId":"Wpy56u2u2b2PDEg42c377Sbhszfdr9Jck2Pvz7KcUP5Rq6m2Z89XlLUfDlpD793DQI0jxzyHYVVz9cXB","body":"Citribel requested what we can offer for the below:\n \n·  Loading: Tienen, BE3300\n·  Delivery: Ripley, DE5 8JZ\n·  Tautliner\n·  No fuel to be applied\n·  Customs done by customer\n·  Volume indications not available\nThank you!","sender":{"emailAddress":"esh4087@truesoldiershop.com","displayName":""},"recipient":[{"emailAddress":"svetikvm@mycbt.me","displayName":""}],"date":"2024-02-19T19:11:11.000Z","subject":"New Shipment Request"}</t>
@@ -2772,30 +2685,6 @@
   <si>
     <t>[
   {
-    "origin_location": "Werk Bobingen, Lindauer Straße 70, 86399 Bobingen",
-    "destination_location": "520077 Sfantu Gheorghe, jud. Covasna",
-    "currency": "EUR",
-    "distance": 0,
-    "transport_type": "FTL",
-    "trailer_type": "13.6 curtain trailer",
-    "dangerous_hazardous": "No",
-    "cargo_type": "General",
-    "steps": [],
-    "validity_date": "",
-    "loading_date": "2024-02-05T00:00:000Z",
-    "arrival_date": "",
-    "weight": 11000,
-    "volume": 0,
-    "pallets": [],
-    "vehicle_loading_method": "vehicle rear loading",
-    "temperature_requirements": [],
-    "seals": false
-  }
-]</t>
-  </si>
-  <si>
-    <t>[
-  {
     "origin_location": "Wetteren",
     "destination_location": "",
     "currency": "EUR",
@@ -2825,59 +2714,6 @@
   <si>
     <t>[
   {
-    "origin_location": "52477 Alsdorf, GERMANY",
-    "destination_location": "5653 LD Eindhoven, Netherlands",
-    "currency": "EUR",
-    "distance": 0,
-    "transport_type": "FTL",
-    "trailer_type": "13.6 curtain trailer",
-    "dangerous_hazardous": "No",
-    "cargo_type": "General",
-    "steps": [],
-    "validity_date": "",
-    "loading_date": "2024-02-09T11:00:000Z",
-    "arrival_date": "2024-02-09T00:00:000Z",
-    "weight": 125,
-    "volume": 0,
-    "pallets": [
-      {
-        "amount": 1,
-        "type": "pallet 800x1200"
-      }
-    ],
-    "vehicle_loading_method": "vehicle rear loading",
-    "temperature_requirements": [],
-    "seals": false
-  }
-]</t>
-  </si>
-  <si>
-    <t>[
-  {
-    "origin_location": "Vreeland 3633",
-    "destination_location": "Falkenberg, Sweden",
-    "currency": "EUR",
-    "distance": 0,
-    "transport_type": "FTL",
-    "trailer_type": "13.6 curtain trailer",
-    "dangerous_hazardous": "No",
-    "cargo_type": "General",
-    "steps": [],
-    "validity_date": "",
-    "loading_date": "2024-01-04T00:00:000Z",
-    "arrival_date": "2024-01-09T00:00:000Z",
-    "weight": 6000,
-    "volume": 0,
-    "pallets": [],
-    "vehicle_loading_method": "vehicle rear loading",
-    "temperature_requirements": [],
-    "seals": false
-  }
-]</t>
-  </si>
-  <si>
-    <t>[
-  {
     "origin_location": "Blästerteknik Gislaved",
     "destination_location": "Sibbhult",
     "currency": "EUR",
@@ -3308,16 +3144,6 @@
   <si>
     <t>[
   {
-    "origin_location": "Werk Bobingen, Lindauer Straße 70, 86399 Bobingen",
-    "destination_location": "520077 Sfantu Gheorghe, jud. Covasna",
-    "loading_date": "2024-02-05T00:00:000Z",
-    "weight": 11000
-  }
-]</t>
-  </si>
-  <si>
-    <t>[
-  {
     "origin_location": "Wetteren",
     "loading_date": "2024-01-15T00:00:000Z",
     "arrival_date": "2024-01-19T00:00:000Z",
@@ -3334,34 +3160,6 @@
   <si>
     <t>[
   {
-    "origin_location": "52477 Alsdorf, GERMANY",
-    "destination_location": "5653 LD Eindhoven, Netherlands",
-    "loading_date": "2024-02-09T11:00:000Z",
-    "arrival_date": "2024-02-09T00:00:000Z",
-    "weight": 125,
-    "pallets": [
-      {
-        "amount": 1,
-        "type": "pallet 800x1200"
-      }
-    ]
-  }
-]</t>
-  </si>
-  <si>
-    <t>[
-  {
-    "origin_location": "Vreeland 3633",
-    "destination_location": "Falkenberg, Sweden",
-    "loading_date": "2024-01-04T00:00:000Z",
-    "arrival_date": "2024-01-09T00:00:000Z",
-    "weight": 6000
-  }
-]</t>
-  </si>
-  <si>
-    <t>[
-  {
     "origin_location": "Blästerteknik Gislaved",
     "destination_location": "Sibbhult",
     "arrival_date": "2024-03-15T00:00:000Z"
@@ -3425,12 +3223,6 @@
     <t>[{"origin_location":"Wetteren","destination_location":"","currency":"EUR","distance":0,"transport_type":"FTL","trailer_type":"13.6 curtain trailer","dangerous_hazardous":"No","cargo_type":"General","steps":[],"validity_date":"","loading_date":"2024-01-15T00:00:000Z","arrival_date":"2024-01-19T00:00:000Z","weight":18270,"volume":0,"pallets":[{"amount":52,"type":"pallet 800x1200"}],"vehicle_loading_method":"vehicle rear loading","temperature_requirements":[],"seals":false}]</t>
   </si>
   <si>
-    <t>[{"origin_location":"52477 Alsdorf, GERMANY","destination_location":"5653 LD Eindhoven, Netherlands","currency":"EUR","distance":0,"transport_type":"FTL","trailer_type":"13.6 curtain trailer","dangerous_hazardous":"No","cargo_type":"General","steps":[],"validity_date":"","loading_date":"2024-02-09T11:00:000Z","arrival_date":"2024-02-09T00:00:000Z","weight":125,"volume":0,"pallets":[{"amount":1,"type":"pallet 800x1200"}],"vehicle_loading_method":"vehicle rear loading","temperature_requirements":[],"seals":false}]</t>
-  </si>
-  <si>
-    <t>[{"origin_location":"Vreeland 3633","destination_location":"Falkenberg, Sweden","currency":"EUR","distance":0,"transport_type":"FTL","trailer_type":"13.6 curtain trailer","dangerous_hazardous":"No","cargo_type":"General","steps":[],"validity_date":"","loading_date":"2024-01-04T00:00:000Z","arrival_date":"2024-01-09T00:00:000Z","weight":6000,"volume":0,"pallets":[],"vehicle_loading_method":"vehicle rear loading","temperature_requirements":[],"seals":false}]</t>
-  </si>
-  <si>
     <t>[{"origin_location":"Blästerteknik Gislaved","destination_location":"Sibbhult","currency":"EUR","distance":0,"transport_type":"FTL","trailer_type":"13.6 curtain trailer","dangerous_hazardous":"No","cargo_type":"General","steps":[],"validity_date":"","loading_date":"","arrival_date":"2024-03-15T00:00:000Z","weight":0,"volume":0,"pallets":[],"vehicle_loading_method":"vehicle rear loading","temperature_requirements":[],"seals":false}]</t>
   </si>
   <si>
@@ -3455,16 +3247,7 @@
     <t>[{"origin_location":"Rotterdam","destination_location":"Bacau","loading_date":"2024-03-22T00:00:000Z","weight":22000,"pallets":[{"amount":20,"type":"pallet 800x1200"}]}]</t>
   </si>
   <si>
-    <t>[{"origin_location":"Werk Bobingen, Lindauer Straße 70, 86399 Bobingen","destination_location":"520077 Sfantu Gheorghe, jud. Covasna","loading_date":"2024-02-05T00:00:000Z","weight":11000}]</t>
-  </si>
-  <si>
     <t>[{"origin_location":"Wetteren","loading_date":"2024-01-15T00:00:000Z","arrival_date":"2024-01-19T00:00:000Z","weight":18270,"pallets":[{"amount":52,"type":"pallet 800x1200"}]}]</t>
-  </si>
-  <si>
-    <t>[{"origin_location":"52477 Alsdorf, GERMANY","destination_location":"5653 LD Eindhoven, Netherlands","loading_date":"2024-02-09T11:00:000Z","arrival_date":"2024-02-09T00:00:000Z","weight":125,"pallets":[{"amount":1,"type":"pallet 800x1200"}]}]</t>
-  </si>
-  <si>
-    <t>[{"origin_location":"Vreeland 3633","destination_location":"Falkenberg, Sweden","loading_date":"2024-01-04T00:00:000Z","arrival_date":"2024-01-09T00:00:000Z","weight":6000}]</t>
   </si>
   <si>
     <t>[{"origin_location":"Blästerteknik Gislaved","destination_location":"Sibbhult","arrival_date":"2024-03-15T00:00:000Z"}]</t>
@@ -3555,6 +3338,341 @@
   </si>
   <si>
     <t>[{"origin_location":"KN Pharma, ALMAC, 9 CHARLESTOWN ROAD, BT63 5QD CRAIGAVON, GB","destination_location":"JANSSEN BELGIUM, RUE DU BOIS DE LA HUTTE 7, 7110 LA LOUVIERE, BE","loading_date":"2024-02-27T08:00:00.000Z","arrival_date":"2024-02-29T09:00:00.000Z"}]</t>
+  </si>
+  <si>
+    <t>{
+  "conversationId": "QzHeJ8GUFLAX1rV89F6M5lxCyG11lSGvoqyxuQhGVlFX4X0Ecv3r0bdTo64LQy4cBiaw4TxCSqGq2elA",
+  "body": "Hello.\nIs it possible to pick up some pallets from Blästerteknik Gislaved to morrow? And deliver it to Sibbhult tomorrow or Monday?",
+  "sender": {
+    "emailAddress": "fjiohio@estudiosucre.com",
+    "displayName": ""
+  },
+  "recipient": [
+    {
+      "emailAddress": "klimenkovmaksim@filevino.com",
+      "displayName": ""
+    }
+  ],
+  "date": "2024-03-14T06:34:11.110Z",
+  "subject": "Pallets from Blästerteknik Gislaved to Sibbhult"
+}</t>
+  </si>
+  <si>
+    <t>{"conversationId":"QzHeJ8GUFLAX1rV89F6M5lxCyG11lSGvoqyxuQhGVlFX4X0Ecv3r0bdTo64LQy4cBiaw4TxCSqGq2elA","body":"Hello.\nIs it possible to pick up some pallets from Blästerteknik Gislaved to morrow? And deliver it to Sibbhult tomorrow or Monday?","sender":{"emailAddress":"fjiohio@estudiosucre.com","displayName":""},"recipient":[{"emailAddress":"klimenkovmaksim@filevino.com","displayName":""}],"date":"2024-03-14T06:34:11.110Z","subject":"Pallets from Blästerteknik Gislaved to Sibbhult"}</t>
+  </si>
+  <si>
+    <t>{"conversationId":"29v8t0ALv4z0os8R8G97A92JnueL23mRzTv9VN6Q72I4y9eTiWb0qCshrp4UxQ6U50tff0vmtZw8r13r","body":"We received RFQ from our automotive customer for below two lines:\nFR-59000 to GB - OX16 4TG, Single trip, Mega trailer, 20 trailers per week.\nGB - OX16 4TG to FR-42230, Single trip, Mega trailer, 15 trailers per week.\n\n Additional details below:\n·         Automotive Customer.\n·         Goods - Automotive Components.\n·         A just-in-time environment.\n·         95% of GPS requirement.\n·         Customs clearance should be on collection sites.\n·         Minimum notification 24h before collection.\n\n Deadline for this RFQ is 26/02/2024.","sender":{"emailAddress":"mark_smith-cargo@domain.com","displayName":"Mark Smith"},"recipient":[{"emailAddress":"cardansgiro@evgeniyvis.com","displayName":""}],"date":"2024-02-11T13:41:06.006Z","subject":"Transportation RFQ from Automotive Customer"}</t>
+  </si>
+  <si>
+    <t>{"conversationId":"9jGfNk68eG0h2Wjlj8wAOdXeNxl36ZtqLGzrFBiC2F6hQ2XIA2Y5TIIb7d3Mz5Dpg1b47TyWZV6Srd5N","body":"2 FTL’s , non haz. Goods are wholesale dry goods.\nStandard curtainsided tautliner is fine\nCollection\nUnit 6, Elm Farm Ind. Estate, Edison Road, Bedford, Bedfordshire MK41 0HR\nDelivery\nCP  30870 Mazarrón\nMurcia - España\n \nFor the customs team:\nIncoterms\nDAP\nAverage number of HS codes (commodity codes) per shipment\n1-3\nOrigin of Goods\nUK\nAre the Goods controlled (require license/additional customs checks)?\nNo\nHave you shipped before\nYes\nProduct type\nToiletries, household cleaning products","sender":{"emailAddress":"dolds2735@newbreedapps.com","displayName":""},"recipient":[{"emailAddress":"keno87@trantienclone.top","displayName":"Ken"}],"date":"2024-02-15T15:41:19.541Z","subject":"New Shipment Request"}</t>
+  </si>
+  <si>
+    <t>{
+  "conversationId": "29v8t0ALv4z0os8R8G97A92JnueL23mRzTv9VN6Q72I4y9eTiWb0qCshrp4UxQ6U50tff0vmtZw8r13r",
+  "body": "We received RFQ from our automotive customer for below two lines:\nFR-59000 to GB - OX16 4TG, Single trip, Mega trailer, 20 trailers per week.\nGB - OX16 4TG to FR-42230, Single trip, Mega trailer, 15 trailers per week.\n\n Additional details below:\n·         Automotive Customer.\n·         Goods - Automotive Components.\n·         A just-in-time environment.\n·         95% of GPS requirement.\n·         Customs clearance should be on collection sites.\n·         Minimum notification 24h before collection.\n\n Deadline for this RFQ is 26/02/2024.",
+  "sender": {
+    "emailAddress": "mark_smith-cargo@domain.com",
+    "displayName": "Mark Smith"
+  },
+  "recipient": [
+    {
+      "emailAddress": "cardansgiro@evgeniyvis.com",
+      "displayName": ""
+    }
+  ],
+  "date": "2024-02-11T13:41:06.006Z",
+  "subject": "Transportation RFQ from Automotive Customer"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "conversationId": "9jGfNk68eG0h2Wjlj8wAOdXeNxl36ZtqLGzrFBiC2F6hQ2XIA2Y5TIIb7d3Mz5Dpg1b47TyWZV6Srd5N",
+  "body": "2 FTL’s , non haz. Goods are wholesale dry goods.\nStandard curtainsided tautliner is fine\nCollection\nUnit 6, Elm Farm Ind. Estate, Edison Road, Bedford, Bedfordshire MK41 0HR\nDelivery\nCP  30870 Mazarrón\nMurcia - España\n \nFor the customs team:\nIncoterms\nDAP\nAverage number of HS codes (commodity codes) per shipment\n1-3\nOrigin of Goods\nUK\nAre the Goods controlled (require license/additional customs checks)?\nNo\nHave you shipped before\nYes\nProduct type\nToiletries, household cleaning products",
+  "sender": {
+    "emailAddress": "dolds2735@newbreedapps.com",
+    "displayName": ""
+  },
+  "recipient": [
+    {
+      "emailAddress": "keno87@trantienclone.top",
+      "displayName": "Ken"
+    }
+  ],
+  "date": "2024-02-15T15:41:19.541Z",
+  "subject": "New Shipment Request"
+}</t>
+  </si>
+  <si>
+    <t>llm_input</t>
+  </si>
+  <si>
+    <t>{"date":"2024-04-01T09:56:01.944Z","sender":{"emailAddress":"jan.kowalski@gmail.com","displayName":"Jan Kowalski"},"subject":"Transport z Krakowa do Katowic","body":"Hej, Musimy dostarczyć część naszego SKU 12345 z Krakowa do Katowic. Odbiór zaplanowano na 5 kwietnia 2024 r. Będzie to 12 palet z 14 tonami produktów. Będą dwa miejsca odbioru, oba w Krakowie. Cała reszta w standardzie. Czekam na wycenę. To, co najlepsze"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-02-02T11:43:01.900Z","sender":{"emailAddress":"tom@oulook.com","displayName":""},"subject":"Quotation request","body":"Buna ziua,\n \nVa rog sa ma ajutati cu o cotatie de transport – 1 camion full, fara ADR, prelata standard, pe ruta 22060 Novedrate (CO) / Italy - 520077 Sfantu Gheorghe (CV) / Romania, marfa generala, avand urmatoarele caracteristici:\nData incarcarii: 19.02.2024\nAdresa de incarcare: 22060 Novedrate (CO), ITALY - avizare furnizor cu 24 de ore inainte\nMarfa: Marfa generala, role de armatura, greutatea totala aprox.15 tone – Nu intra in categoria BRFR\nIncarcare/descarcare pe laterale.\nTermen de plata 45 zile de la data facturii.\nLoc descarcare: Sika Romania srl. – fabrica de membrane\n520077 Sfantu Gheorghe, jud. Covasna , program : 08:00-15:00\nMultumesc.\nCu stima,"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-02-11T14:11:04.400Z","sender":{"emailAddress":"tom@oulook.com","displayName":""},"subject":"Quotation request","body":"Buna ziua ,\n \nVa rog o cotatie pentru acest grupaj :\n \n   Incarcare 15.02.  Lehliu-gara ,\n    Str Crinului nr 1 .\n\t915300,   jud Calarasi\n \nAdresa de descarcare:\n\n\n\n10 paleti 80x120x260cm Greutate totala 3500 kg .\n \nCand ne trimiteti oferta sa imi dati va rog si data de descarcare ."}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-15T14:08:32.432Z","sender":{"emailAddress":"onufrienkonikita@mainetaxicab.com","displayName":""},"subject":"Transport panouri fotovoltaice din Rotterdam la Bacau","body":"Buna Radu,\nCat ar costa acum un camion din Rotterdam, cu prelata, 22 tone 20 paleti panouri fotovoltaice cu descarcare la Bacau ? (incarcare in 1-2 saptamani)\nMultumesc!"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-15T14:08:32.432Z","sender":{"emailAddress":"ardentrans@bankcommon.com","displayName":""},"subject":"","body":"Buna,\n \nVa rog sa ne ajuti cu o cotatie de transport pentru 3 paleti - suplimente alimentare, greutate bruta – 458Kg, 120x100x133, luand in considerare urmatoarele:\nExport UK si control sanitar veterinar in Calais, Franta -  in sarcina IB Cargo (DVE + T1);\nControl sanitar veterninar la Calais in sarcina Prisum;\nVama import Otopeni in sarcina Prisum;\nTaxe vamale si TVA in vama la import in sarcina Prisum.\n \nAdresa de incarcare:\nUnit 1 Bridgwater Trade Park.\nA38 Bristol Road,\nBridgwater\nTA6 4WA (or driver can type Easy Bathrooms &amp; Tiles Bridgwater on google maps and our warehouse is near this store)\nProgram depozit: 08.00 – 16.30\nReferinta incarcare: 111681\n"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-01-13T06:32:44.043Z","sender":{"emailAddress":"pde6868@bestmms.cloud","displayName":""},"subject":"Transport TURCIA - ROMANIA","body":"Buna ziua\nVa rog ma ajutati cu o cotatie  de pret  pentru un transport din TURCIA:\n \nUn palet tabla inox-1035 kg\n \nexp:\nLoading Address:\nTeknik Metal A.S.\nOsmangazi Mah. 3143 sok. No: 7 Esenyurt Istanbul Turkey 34522\nContact person: Serdar Yeşilkaya\n+90 212 665 0404\n \nGoogle maps:\nhttps://goo.gl/maps/CuuqUxkJGXz\n\n\n\n\ndest:\nSC KOBER SRL SUCURSALA VADURI Com Alexandru  Cel Bun,  CP 617511 str ZORELELOR 25 LOCALITATE VADURI, JUD NEAMT, ROMANIA\nMultumesc.\n"}</t>
+  </si>
+  <si>
+    <t>{"date":"2023-12-30T11:43:01.000Z","sender":{"emailAddress":"kcolli1221@dnult.xyz","displayName":"Dunlt"},"subject":"Cotatie de pret transport Germania - Romania","body":"Buna ziua,\n \nVa rog sa ne comunicati o cotatie de pret pentru 1 camion complet, non ADR, transport pe ruta  Germania  – Romania in urmatoarele conditii:\nData incarcarii: 05.02.2024\nWerk Bobingen                                    \nLindauer Straße 70                             \n86399 Bobingen\n \nLoading time\nMonday – Thursday 7:00 am – 2:00 pm\nFriday 7:00 am – 1:00 pm\n(the truck should arrive 1 hour before closing for cargo)\n \n \nBefore collection: Please contact our warehouse in order to agree the exact date and details of the pick-up.\nShould the truck arrive unannounced, please consider a longer waiting time.\n \n \nMarfa: generala 22 paleti cu 44 role / camion , 11 tone – armatura de poliester - NU este marfa cu risc fiscal ridicat\n \nLocalitate descarcare: 520077 Sfantu Gheorghe , jud. Covasna , program : 08:00-15:00\n \nTermen de plata 45 zile.\n \nCamioanele trebuie sa fie dotate cu certificat XL valabil la data incarcarii.\n! Exclus semiremorci fara certificat XL!\n \nMultumesc."}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-01-04T09:22:01.000Z","sender":{"emailAddress":"rujma@bankinnepal.com","displayName":""},"subject":"","body":"Buna ziua,\nVa rog sa-mi transmiteti oferta dvs, de transport, in grupaj, pentru:\n1 palet: 120cm x 80cm x 120cm – greutate aprox 155 Kg\nIncarcare: 300283 Timisoara, Romania\nDescarcare: 4715-405 Braga, Portugalia\nSe poate ridica. Plata la 7 zile"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-11T17:01:22.430Z","sender":{"emailAddress":"tjmbpc2@nhancodelienquan.com","displayName":""},"subject":"","body":"Buna ziua,\n \nVa rog sa-mi transmiteti cea mai buna cotatie de pret pentru incarcarea din Wetteren:\n \nData de incarcare :  15/01/2024\n \nCantitate: 52 palleti industriali suprapozabili - 1 camion\nGreutate: gross 18,270 kg\n \nData de descarcare : 19/01/2024\n \n \nMultumesc,"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-02-07T14:53:11.421Z","sender":{"emailAddress":"saralee5@sentimentdate.com","displayName":"Sara Lee"},"subject":"","body":"Beste,\nGraag prijs maken voor het volgende transport. the reference number for pickup is: RF2402080145TP_AF\nPickup 09/02 om 11:00-delivery 09/02 rechtstreeks\nGraag prijs aanbieden vóór 09/02 om 08:00\nFrom:\n52477 Alsdorf GERMANY\n1 kist 80x70x60-125 kg\nTo:\nPanch Powertrain-t\n5653 LD Eindhoven\nNetherlands"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-01-01T15:01:44.000Z","sender":{"emailAddress":"osu2005@hulas.us","displayName":""},"subject":"Vreeland - Falkenberg","body":"Goedemorgen Bart,\nWat is jullie tarief voor laden 04.01 in Vreeland 3633 en leveren 09.01 in Falkenberg Zweden\nFTL, lege nieuwe vaten, rond 5-6t\nPallets 274cm hoog!\n"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-14T06:34:11.110Z","sender":{"emailAddress":"fjiohio@estudiosucre.com","displayName":""},"subject":"Pallets from Blästerteknik Gislaved to Sibbhult","body":"Hello.\nIs it possible to pick up some pallets from Blästerteknik Gislaved to morrow? And deliver it to Sibbhult tomorrow or Monday?"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-01-09T11:59:11.000Z","sender":{"emailAddress":"ambrodel@code-gmail.com","displayName":""},"subject":"Vracht naar VW Poznan Werk Wrzesnia","body":"Hallo,\nKunnen jullie voor maandag 12/02 een vracht regelen naar onderstaan adres:\nVW Poznan Werk Wrzesnia\nBiałężyce 100\n62-300 Wrzesnia\nLading is 2 dozen 2m*2m*1m\nGewicht is ongeveer 1000kg\nVracht kan afgehaald worden vanaf 8u30\nMet vriendelijke groeten,\nJan"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-05T11:44:22.333","sender":{"emailAddress":"valuchka@cnuwim.com","displayName":""},"subject":"Price request for Monday 11th March","body":"Good morning,\nCan you please price the below for loading Monday:\nAlfreton – Wimille FR (please price standard AND MEGA if available) 450e standard / 50e mega\nEdmonton – Den Ham NL – 600e mega\nBarnsley – Ardooie BE 550e mega\nWest Bromwich – Raubach DE  -  900e\nHoddesdon – Bottrop DE – 600e mega\nHoddesdon – Den Ham NL - 600e mega\nBarnsley – 25813 Husum DE – 1,600e mega\nWitham – Ham BE – 395e mega"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-23T16:03:01.129","sender":{"emailAddress":"mart1958@hulas.us","displayName":"Martina"},"subject":"Potain Manitowoc - Quote needed for below lanes","body":"Potain Manitowoc needs to have below lanes quoted.\nExecution : April / may 2024\nAbout 10-13 shipments with mix of tautliners and flatbeds\nFrom Avermes FR03000 to Avonmouth Bristol BS11 9DQ\nFrom Avermes FR03000 to Buckingham GB MK18 4FD\nFrom Buckingham GB MK18 4FD to Avonmouth Bristol BS11 9DQ"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-18T07:53:56.103Z","sender":{"emailAddress":"rmsabo@greenpanel.xyz","displayName":""},"subject":"","body":"Can you please price:\nAlfreton – 5667 KX Geldrop NL\nAndover – Nivelles BE\nMany thanks.\n"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-02-11T13:41:06.006Z","sender":{"emailAddress":"mark_smith-cargo@domain.com","displayName":"Mark Smith"},"subject":"Transportation RFQ from Automotive Customer","body":"We received RFQ from our automotive customer for below two lines:\nFR-59000 to GB - OX16 4TG, Single trip, Mega trailer, 20 trailers per week.\nGB - OX16 4TG to FR-42230, Single trip, Mega trailer, 15 trailers per week.\n\n Additional details below:\n·         Automotive Customer.\n·         Goods - Automotive Components.\n·         A just-in-time environment.\n·         95% of GPS requirement.\n·         Customs clearance should be on collection sites.\n·         Minimum notification 24h before collection.\n\n Deadline for this RFQ is 26/02/2024."}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-02-15T15:41:19.541Z","sender":{"emailAddress":"dolds2735@newbreedapps.com","displayName":""},"subject":"New Shipment Request","body":"2 FTL’s , non haz. Goods are wholesale dry goods.\nStandard curtainsided tautliner is fine\nCollection\nUnit 6, Elm Farm Ind. Estate, Edison Road, Bedford, Bedfordshire MK41 0HR\nDelivery\nCP  30870 Mazarrón\nMurcia - España\n \nFor the customs team:\nIncoterms\nDAP\nAverage number of HS codes (commodity codes) per shipment\n1-3\nOrigin of Goods\nUK\nAre the Goods controlled (require license/additional customs checks)?\nNo\nHave you shipped before\nYes\nProduct type\nToiletries, household cleaning products"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-02-19T19:11:11.000Z","sender":{"emailAddress":"esh4087@truesoldiershop.com","displayName":""},"subject":"New Shipment Request","body":"Citribel requested what we can offer for the below:\n \n·  Loading: Tienen, BE3300\n·  Delivery: Ripley, DE5 8JZ\n·  Tautliner\n·  No fuel to be applied\n·  Customs done by customer\n·  Volume indications not available\nThank you!"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-01T06:00:00.000","sender":{"emailAddress":"mjmck3@villastream.xyz","displayName":""},"subject":"Quote Request","body":"Could you please quote the lanes below.\nDeparture:\nKreidewerk Rügen\nKlementelvitz\n18546\nSassnitz\nGermany\nFor delivery to the following postcodes in UK:\nAB54\nDG2\nLL60\nML11\nSA60\nSA66\nSY23\nAdditionally could you add Transit Time for each lane."}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-16T06:06:55.000","sender":{"emailAddress":"martindm3@nktechnical.tech","displayName":"Martin D. M."},"subject":"","body":"Hello,\nCan you please give me a price and please check whether we can make the loading today?\nCHESHIRE CW5 6RS United Kingdom to 2742 RH Waddinxveen Netherlands,  Gross weight 4,406.40 and 6 pallets.\nBest regards,"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-01-06T08:34:32.111","sender":{"emailAddress":"hungrydemon@kintamaw.click","displayName":"Hungry"},"subject":"Quotation Request from Cyprus to Milano","body":"Dear Sandro,\n \nCan you please quote for the below from Cyprus to Milano area ?\n \nAddress :             Limassol, Cyprus\n \nFrom 1/3 plts\n4/6 plts\n7/10 plts\n11/16 plts\n16/20 plts\n21/33 plts\n \nPharma\n \nSet temp + 15"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-01T05:11:54.000Z","sender":{"emailAddress":"kissantassu@shopbantkclone.com","displayName":""},"subject":"Request","body":"Hello\n \nPlease can you add the below to the rate card?\n \nB.BRAUN LOGISTICS, S. L.\n  CALLE MONTMELL, PARCELAS 4 Y 7\n  POLÍGONO INDUSTRIAL ALBORNAR 2, SANTA OLIVA\n  43710 TARRAGONA\n  ES\n \nALLOGA FRANCE\n  AVENUE DE L’ETOILE DU SUD POLE JULES VERNE 20,\n  ZI LA CROIX DE FER,\n  80440 GLISY\n  FR\n"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-02T07:31:22.000Z","sender":{"emailAddress":"gribow84@dubukim.me","displayName":""},"subject":"","body":"Please can you add the below onto the ratecard?\n \nPick-up address\nCompany\nID Logistics Iberia S.A. La Granada\nAvinguda Alt Penedes S/N nav.\n08792 LA GRANADA\nSPAIN\nContact:\nT: +340936401516\n \nDelivery address\nBrocacef NL HUB\nBasicweg 8\n3800 CA POTSBUS 2232 ,AMERSFOORT\nNETHERLANDS\n"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-11T16:22:18.987Z","sender":{"emailAddress":"koshkamioshka@danoshass.cloud","displayName":"Koshka Mioshka"},"subject":"Request for a quote for a dedicated truck vs groupage from Bari to Turkey","body":"Dear Essers team\n \nCan you please provide me with the cost difference (per pallet) of a dedicated truck vs groupage leaving from Bari Italy to Turkey?\nThank you in advance,\n \n \n6 palletten, 120 x 80 x 123 max\nAfhaaladres:\nAminolabs\nKiewitstraat 176\nBE-3500 Hasselt\n \nLeveradres :\nChiesi España\nMovianto Spain SLU / Helena Rubinstein 4\n28906 Getafe\nESP"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-02-24T07:12:49.753Z","sender":{"emailAddress":"pickus@nedaned.cloud","displayName":""},"subject":"Vaste tarieven voor temperatuur controlled transport?","body":"Hey,\n \nIs het mogelijk om vaste tarieven te krijgen voor onderstaande business?\nAlle temperatuur controlled transport tussen 15°C en 25°C\n \n \n1 pal naar DE-76646 Bruchsal : +/- 15 keer per jaar\nDE-33729 Bielefeld : we plannen 5 tot 7 shipments voor de rest van 2024 / sealed truck vereist! – alleen dedicated transport + slot boeken in Cargoclix\nPrijs tot  8 pal\nPrijs tot 18 pal\nNO-2016 Frogner (customs formalities required): we plannen om  5 tot 7 shipments te hebben in 2024\nGroupage of dedicated : 3 pal\nGroupage of dedicated : 8 pal\nFTL : 33 pal dedicated (zullen 2 shipments zijn)\nIT-26814 Livraga (LO)\nFTL : 33 pal dedicated (zullen 2 of 3 trucks per maand zijn)\nWe plannen om 20 trucks te versturen naar Italië in 2024."}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-02-11T11:43:00.000Z","sender":{"emailAddress":"dac7423@code-gmail.com","displayName":""},"subject":"Quote request","body":" \nCan you sent me a quote for:\n \n4pll\n951,32kg\n4,640cbm\n \nGDP\nVaccines\n2-8ºC\n \nShipper:\nGlaxoSmithKline Biologicals SA\nRue de l'Institut, 89\nB - 1330 Rixensart\nBelgium\n \nPlace of delivery:\nShip-to Location Name: Farmasoft, LLC\nStreet Name: Boryspolskaya\nStreet Location Number: 9\nPostal Code or PO Box: 08320\nCity: Velyka Oleksandrivka village, Boryspol district, Kyiv region\nCountry: Ukraine"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-02-20T08:17:10.555Z","sender":{"emailAddress":"fedjy@topnnov.ru","displayName":""},"subject":"KN Pharma - 27-02-2024 08:00 - 29-02-2024 09:00 - FTL AL","body":"Hey\n \nKunnen jullie mij de prijs doorgeven van deze aub?\nKN Pharma\nShipFrom\n1\n\nALMAC\n\n\n9 CHARLESTOWN ROAD\n\n\nBT63 5QD CRAIGAVON\nGB\n\n\n\n27-02-2024 08:00\nEurope/London\nShipTo\n2\n\nJANSSEN BELGIUM\n\n\nRUE DU BOIS DE LA HUTTE 7\n\n\n7110 LA LOUVIERE\nBE\n\n\n\n29-02-2024 09:00\nEurope/Brussels\n\nFTL AL"}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-01-20T15:22:33.533Z","sender":{"emailAddress":"1jack@giayhieucu.com","displayName":""},"subject":"Transport request - empty boxes from Softbox NL (AMS) to SOFRIGAM France","body":"We would like to request a price for the transport of empty boxes from Softbox NL (AMS) to\n \nSOFRIGAM France\n98, Allee du Danemark\n62118 Monchy le Preux\nFrance\n \n+/- 12 trucks in total, divided over multiple days TBD. Transport is not confirmed yet."}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-03-24T12:00:53.983Z","sender":{"emailAddress":"brampollers@chickenbell.shop","displayName":"Bram Pollers"},"subject":"Transport request - empty boxes from Softbox NL (AMS) to SOFRIGAM France","body":"Could you please advise the rate for this shipment? \n\nFrom Torre Annunziata IT to crossdock Siziano to Genk = LTL \nFrom Genk to Tampere FI = FTL \n\nPlease advise the rates per shipment as well. Kind regards, \n\nBRAM POLLERS \nSenior Manager Healthcare LLP \nT +32 89 369 453 | M +32 493 319 351"}</t>
+  </si>
+  <si>
+    <t>{
+  "conversationId": "gWuIPOjl3ke4r4gx6GOEV5UFu6q46pmQYwsID7vo7UpABLq51C6yVYtqT8BxrmL7Oq27on3YI8nDomEl",
+  "body": "Buna ziua ,\n \nPermiteti-mi sa revin la solicitarea de oferta  pret pentru un transport despre care am discutat anul trecut .\n“Rog oferta dumneavoastra de pret pentru un transport de 17,00 TO  marfa amablaj ( folii de plastic care folosim ptr impachetarea sacilor de ingrasaminte de 50 kg. ) pentru ruta depozit Fratesti/Giurgiu la  HU- 3580 Tiszaujváros .\nTransportul nu este un camion complet de 24 TO”\n \n \nDe data asta am gasit o varinata sa ducem marfa cu transport international  in Italia.\nDeci ruta este intre  RO - 080557 Giurgiu, Jud. Giurgiu si  IT - 48100 Ravenna.\n \nData exacta la incarcare depinde si de oferta transportatoriului, cum am mentionat si in convorbirile nostre din anul trrecut , trebuie sa facem pregatirile pentru ridicarea marfii si din punct de vedere administrativ.\n \nVa rog sa ma ajutati prin contactele dumneavoastra sa pot organiza acest transport international cat de curand .\n \n \nMultumesc anticipat",
+  "sender": {
+    "emailAddress": "di53a@jualcloud.net",
+    "displayName": ""
+  },
+  "recipient": [
+    {
+      "emailAddress": "contactjosegaytan@elinore1818.site",
+      "displayName": ""
+    }
+  ],
+  "date": "2024-02-24T16:11:32.511Z",
+  "subject": ""
+}</t>
+  </si>
+  <si>
+    <t>{"conversationId":"gWuIPOjl3ke4r4gx6GOEV5UFu6q46pmQYwsID7vo7UpABLq51C6yVYtqT8BxrmL7Oq27on3YI8nDomEl","body":"Buna ziua ,\n \nPermiteti-mi sa revin la solicitarea de oferta  pret pentru un transport despre care am discutat anul trecut .\n“Rog oferta dumneavoastra de pret pentru un transport de 17,00 TO  marfa amablaj ( folii de plastic care folosim ptr impachetarea sacilor de ingrasaminte de 50 kg. ) pentru ruta depozit Fratesti/Giurgiu la  HU- 3580 Tiszaujváros .\nTransportul nu este un camion complet de 24 TO”\n \n \nDe data asta am gasit o varinata sa ducem marfa cu transport international  in Italia.\nDeci ruta este intre  RO - 080557 Giurgiu, Jud. Giurgiu si  IT - 48100 Ravenna.\n \nData exacta la incarcare depinde si de oferta transportatoriului, cum am mentionat si in convorbirile nostre din anul trrecut , trebuie sa facem pregatirile pentru ridicarea marfii si din punct de vedere administrativ.\n \nVa rog sa ma ajutati prin contactele dumneavoastra sa pot organiza acest transport international cat de curand .\n \n \nMultumesc anticipat","sender":{"emailAddress":"di53a@jualcloud.net","displayName":""},"recipient":[{"emailAddress":"contactjosegaytan@elinore1818.site","displayName":""}],"date":"2024-02-24T16:11:32.511Z","subject":""}</t>
+  </si>
+  <si>
+    <t>{"date":"2024-02-24T16:11:32.511Z","sender":{"emailAddress":"di53a@jualcloud.net","displayName":""},"subject":"","body":"Buna ziua ,\n \nPermiteti-mi sa revin la solicitarea de oferta  pret pentru un transport despre care am discutat anul trecut .\n“Rog oferta dumneavoastra de pret pentru un transport de 17,00 TO  marfa amablaj ( folii de plastic care folosim ptr impachetarea sacilor de ingrasaminte de 50 kg. ) pentru ruta depozit Fratesti/Giurgiu la  HU- 3580 Tiszaujváros .\nTransportul nu este un camion complet de 24 TO”\n \n \nDe data asta am gasit o varinata sa ducem marfa cu transport international  in Italia.\nDeci ruta este intre  RO - 080557 Giurgiu, Jud. Giurgiu si  IT - 48100 Ravenna.\n \nData exacta la incarcare depinde si de oferta transportatoriului, cum am mentionat si in convorbirile nostre din anul trrecut , trebuie sa facem pregatirile pentru ridicarea marfii si din punct de vedere administrativ.\n \nVa rog sa ma ajutati prin contactele dumneavoastra sa pot organiza acest transport international cat de curand .\n \n \nMultumesc anticipat"}</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "origin_location": "Werk Bobingen, Lindauer Straße 70, 86399 Bobingen",
+    "destination_location": "520077 Sfantu Gheorghe, jud. Covasna",
+    "currency": "EUR",
+    "distance": 0,
+    "transport_type": "FTL",
+    "trailer_type": "13.6 curtain trailer",
+    "dangerous_hazardous": "No",
+    "cargo_type": "General",
+    "steps": [],
+    "validity_date": "",
+    "loading_date": "2024-02-05T00:00:000Z",
+    "arrival_date": "",
+    "weight": 11000,
+    "volume": 0,
+    "pallets": [
+      {
+        "amount": 22,
+        "type": "pallet 800x1200"
+      }
+    ],
+    "vehicle_loading_method": "vehicle rear loading",
+    "temperature_requirements": [],
+    "seals": false
+  }
+]</t>
+  </si>
+  <si>
+    <t>[{"origin_location":"Werk Bobingen, Lindauer Straße 70, 86399 Bobingen","destination_location":"520077 Sfantu Gheorghe, jud. Covasna","currency":"EUR","distance":0,"transport_type":"FTL","trailer_type":"13.6 curtain trailer","dangerous_hazardous":"No","cargo_type":"General","steps":[],"validity_date":"","loading_date":"2024-02-05T00:00:000Z","arrival_date":"","weight":11000,"volume":0,"pallets":[{"amount":22,"type":"pallet 800x1200"}],"vehicle_loading_method":"vehicle rear loading","temperature_requirements":[],"seals":false}]</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "origin_location": "Werk Bobingen, Lindauer Straße 70, 86399 Bobingen",
+    "destination_location": "520077 Sfantu Gheorghe, jud. Covasna",
+    "loading_date": "2024-02-05T00:00:000Z",
+    "weight": 11000,
+    "pallets": [
+      {
+        "amount": 22,
+        "type": "pallet 800x1200"
+      }
+    ]
+  }
+]</t>
+  </si>
+  <si>
+    <t>[{"origin_location":"Werk Bobingen, Lindauer Straße 70, 86399 Bobingen","destination_location":"520077 Sfantu Gheorghe, jud. Covasna","loading_date":"2024-02-05T00:00:000Z","weight":11000,"pallets":[{"amount":22,"type":"pallet 800x1200"}]}]</t>
+  </si>
+  <si>
+    <t>[{"origin_location":"52477 Alsdorf, GERMANY","destination_location":"5653 LD Eindhoven, Netherlands","currency":"EUR","distance":0,"transport_type":"FTL","trailer_type":"13.6 curtain trailer","dangerous_hazardous":"No","cargo_type":"General","steps":[],"validity_date":"","loading_date":"2024-02-09T11:00:000Z","arrival_date":"2024-02-09T00:00:000Z","weight":125,"volume":0,"pallets":[{"amount":1,"type":"pallet 80x70x60"}],"vehicle_loading_method":"vehicle rear loading","temperature_requirements":[],"seals":false}]</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "origin_location": "52477 Alsdorf, GERMANY",
+    "destination_location": "5653 LD Eindhoven, Netherlands",
+    "currency": "EUR",
+    "distance": 0,
+    "transport_type": "FTL",
+    "trailer_type": "13.6 curtain trailer",
+    "dangerous_hazardous": "No",
+    "cargo_type": "General",
+    "steps": [],
+    "validity_date": "",
+    "loading_date": "2024-02-09T11:00:000Z",
+    "arrival_date": "2024-02-09T00:00:000Z",
+    "weight": 125,
+    "volume": 0,
+    "pallets": [
+      {
+        "amount": 1,
+        "type": "pallet 80x70x60"
+      }
+    ],
+    "vehicle_loading_method": "vehicle rear loading",
+    "temperature_requirements": [],
+    "seals": false
+  }
+]</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "origin_location": "52477 Alsdorf, GERMANY",
+    "destination_location": "5653 LD Eindhoven, Netherlands",
+    "loading_date": "2024-02-09T11:00:000Z",
+    "arrival_date": "2024-02-09T00:00:000Z",
+    "weight": 125,
+    "pallets": [
+      {
+        "amount": 1,
+        "type": "pallet 80x70x60"
+      }
+    ]
+  }
+]</t>
+  </si>
+  <si>
+    <t>[{"origin_location":"52477 Alsdorf, GERMANY","destination_location":"5653 LD Eindhoven, Netherlands","loading_date":"2024-02-09T11:00:000Z","arrival_date":"2024-02-09T00:00:000Z","weight":125,"pallets":[{"amount":1,"type":"pallet 80x70x60"}]}]</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "origin_location": "Vreeland 3633",
+    "destination_location": "Falkenberg, Sweden",
+    "currency": "EUR",
+    "distance": 0,
+    "transport_type": "FTL",
+    "trailer_type": "13.6 curtain trailer",
+    "dangerous_hazardous": "No",
+    "cargo_type": "General",
+    "steps": [],
+    "validity_date": "",
+    "loading_date": "2024-01-04T00:00:000Z",
+    "arrival_date": "2024-01-09T00:00:000Z",
+    "weight": 6000,
+    "volume": 0,
+    "pallets": [
+      {
+        "amount": 1,
+        "type": "pallet1160x2200"
+      }
+    ],
+    "vehicle_loading_method": "vehicle rear loading",
+    "temperature_requirements": [],
+    "seals": false
+  }
+]</t>
+  </si>
+  <si>
+    <t>[{"origin_location":"Vreeland 3633","destination_location":"Falkenberg, Sweden","currency":"EUR","distance":0,"transport_type":"FTL","trailer_type":"13.6 curtain trailer","dangerous_hazardous":"No","cargo_type":"General","steps":[],"validity_date":"","loading_date":"2024-01-04T00:00:000Z","arrival_date":"2024-01-09T00:00:000Z","weight":6000,"volume":0,"pallets":[{"amount":1,"type":"pallet1160x2200"}],"vehicle_loading_method":"vehicle rear loading","temperature_requirements":[],"seals":false}]</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "origin_location": "Vreeland 3633",
+    "destination_location": "Falkenberg, Sweden",
+    "loading_date": "2024-01-04T00:00:000Z",
+    "arrival_date": "2024-01-09T00:00:000Z",
+    "weight": 6000,
+    "pallets": [
+      {
+        "amount": 1,
+        "type": "pallet1160x2200"
+      }
+    ]
+  }
+]</t>
+  </si>
+  <si>
+    <t>[{"origin_location":"Vreeland 3633","destination_location":"Falkenberg, Sweden","loading_date":"2024-01-04T00:00:000Z","arrival_date":"2024-01-09T00:00:000Z","weight":6000,"pallets":[{"amount":1,"type":"pallet1160x2200"}]}]</t>
   </si>
 </sst>
 </file>
@@ -3809,10 +3927,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3820,44 +3938,47 @@
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1"/>
+    <col min="4" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F1" t="s">
         <v>138</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>139</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>140</v>
       </c>
-      <c r="D1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>141</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>142</v>
       </c>
-      <c r="G1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I1" t="s">
-        <v>145</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3868,25 +3989,28 @@
         <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
-        <v>241</v>
-      </c>
       <c r="G2" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="H2" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="I2" t="s">
-        <v>278</v>
+        <v>252</v>
+      </c>
+      <c r="J2" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3897,25 +4021,28 @@
         <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>242</v>
-      </c>
       <c r="G3" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
       <c r="H3" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="I3" t="s">
-        <v>279</v>
+        <v>253</v>
+      </c>
+      <c r="J3" t="s">
+        <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3926,25 +4053,28 @@
         <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>243</v>
-      </c>
       <c r="G4" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="H4" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="I4" t="s">
-        <v>280</v>
+        <v>254</v>
+      </c>
+      <c r="J4" t="s">
+        <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3955,25 +4085,28 @@
         <v>122</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
-        <v>244</v>
-      </c>
       <c r="G5" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
       <c r="H5" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="I5" t="s">
-        <v>281</v>
+        <v>255</v>
+      </c>
+      <c r="J5" t="s">
+        <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3984,25 +4117,28 @@
         <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E6" t="s">
+        <v>303</v>
+      </c>
+      <c r="F6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>103</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4010,28 +4146,31 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>329</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>330</v>
       </c>
       <c r="E7" t="s">
+        <v>331</v>
+      </c>
+      <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>105</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>101</v>
       </c>
@@ -4039,28 +4178,31 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D8" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E8" t="s">
+        <v>304</v>
+      </c>
+      <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>19</v>
       </c>
-      <c r="G8" t="s">
-        <v>310</v>
-      </c>
       <c r="H8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I8" t="s">
         <v>107</v>
       </c>
-      <c r="I8" t="s">
-        <v>309</v>
+      <c r="J8" t="s">
+        <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4068,28 +4210,31 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E9" t="s">
+        <v>305</v>
+      </c>
+      <c r="F9" t="s">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
-        <v>245</v>
-      </c>
       <c r="G9" t="s">
-        <v>259</v>
+        <v>332</v>
       </c>
       <c r="H9" t="s">
-        <v>127</v>
+        <v>334</v>
       </c>
       <c r="I9" t="s">
-        <v>282</v>
+        <v>333</v>
+      </c>
+      <c r="J9" t="s">
+        <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -4097,28 +4242,31 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E10" t="s">
+        <v>306</v>
+      </c>
+      <c r="F10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>25</v>
       </c>
-      <c r="H10" t="s">
-        <v>128</v>
-      </c>
       <c r="I10" t="s">
-        <v>129</v>
+        <v>126</v>
+      </c>
+      <c r="J10" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -4126,28 +4274,31 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E11" t="s">
+        <v>307</v>
+      </c>
+      <c r="F11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" t="s">
-        <v>246</v>
-      </c>
       <c r="G11" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="H11" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="I11" t="s">
-        <v>283</v>
+        <v>256</v>
+      </c>
+      <c r="J11" t="s">
+        <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -4155,28 +4306,31 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E12" t="s">
+        <v>308</v>
+      </c>
+      <c r="F12" t="s">
         <v>30</v>
       </c>
-      <c r="F12" t="s">
-        <v>247</v>
-      </c>
       <c r="G12" t="s">
-        <v>261</v>
+        <v>337</v>
       </c>
       <c r="H12" t="s">
-        <v>272</v>
+        <v>338</v>
       </c>
       <c r="I12" t="s">
-        <v>284</v>
+        <v>336</v>
+      </c>
+      <c r="J12" t="s">
+        <v>339</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -4184,28 +4338,31 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D13" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E13" t="s">
+        <v>309</v>
+      </c>
+      <c r="F13" t="s">
         <v>30</v>
       </c>
-      <c r="F13" t="s">
-        <v>248</v>
-      </c>
       <c r="G13" t="s">
-        <v>262</v>
+        <v>340</v>
       </c>
       <c r="H13" t="s">
-        <v>273</v>
+        <v>342</v>
       </c>
       <c r="I13" t="s">
-        <v>285</v>
+        <v>341</v>
+      </c>
+      <c r="J13" t="s">
+        <v>343</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -4213,28 +4370,31 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>292</v>
       </c>
       <c r="D14" t="s">
-        <v>214</v>
+        <v>293</v>
       </c>
       <c r="E14" t="s">
+        <v>310</v>
+      </c>
+      <c r="F14" t="s">
         <v>34</v>
       </c>
-      <c r="F14" t="s">
-        <v>249</v>
-      </c>
       <c r="G14" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="H14" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="I14" t="s">
-        <v>286</v>
+        <v>257</v>
+      </c>
+      <c r="J14" t="s">
+        <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -4242,28 +4402,31 @@
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D15" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E15" t="s">
+        <v>311</v>
+      </c>
+      <c r="F15" t="s">
         <v>30</v>
       </c>
-      <c r="F15" t="s">
-        <v>250</v>
-      </c>
       <c r="G15" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="H15" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="I15" t="s">
-        <v>287</v>
+        <v>258</v>
+      </c>
+      <c r="J15" t="s">
+        <v>267</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -4271,28 +4434,31 @@
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E16" t="s">
+        <v>312</v>
+      </c>
+      <c r="F16" t="s">
         <v>34</v>
       </c>
-      <c r="F16" t="s">
-        <v>251</v>
-      </c>
       <c r="G16" t="s">
-        <v>162</v>
+        <v>239</v>
       </c>
       <c r="H16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I16" t="s">
-        <v>163</v>
+        <v>156</v>
+      </c>
+      <c r="J16" t="s">
+        <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -4300,28 +4466,31 @@
         <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D17" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E17" t="s">
+        <v>313</v>
+      </c>
+      <c r="F17" t="s">
         <v>34</v>
       </c>
-      <c r="F17" t="s">
-        <v>252</v>
-      </c>
       <c r="G17" t="s">
-        <v>165</v>
+        <v>240</v>
       </c>
       <c r="H17" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I17" t="s">
-        <v>166</v>
+        <v>159</v>
+      </c>
+      <c r="J17" t="s">
+        <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -4329,28 +4498,31 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D18" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="E18" t="s">
+        <v>314</v>
+      </c>
+      <c r="F18" t="s">
         <v>34</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>40</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>41</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>108</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -4358,57 +4530,63 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>296</v>
       </c>
       <c r="D19" t="s">
-        <v>219</v>
+        <v>294</v>
       </c>
       <c r="E19" t="s">
+        <v>315</v>
+      </c>
+      <c r="F19" t="s">
         <v>34</v>
       </c>
-      <c r="F19" t="s">
-        <v>253</v>
-      </c>
       <c r="G19" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="H19" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="I19" t="s">
-        <v>288</v>
+        <v>259</v>
+      </c>
+      <c r="J19" t="s">
+        <v>268</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>155</v>
+        <v>297</v>
       </c>
       <c r="D20" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
       <c r="E20" t="s">
+        <v>316</v>
+      </c>
+      <c r="F20" t="s">
         <v>34</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>43</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>44</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>110</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -4416,28 +4594,31 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E21" t="s">
+        <v>317</v>
+      </c>
+      <c r="F21" t="s">
         <v>34</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>46</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>47</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>112</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -4445,28 +4626,31 @@
         <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D22" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E22" t="s">
+        <v>318</v>
+      </c>
+      <c r="F22" t="s">
         <v>34</v>
       </c>
-      <c r="F22" t="s">
-        <v>169</v>
-      </c>
       <c r="G22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H22" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="I22" t="s">
-        <v>168</v>
+        <v>165</v>
+      </c>
+      <c r="J22" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -4474,57 +4658,63 @@
         <v>49</v>
       </c>
       <c r="C23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D23" t="s">
+        <v>214</v>
+      </c>
+      <c r="E23" t="s">
+        <v>319</v>
+      </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" t="s">
+        <v>242</v>
+      </c>
+      <c r="H23" t="s">
+        <v>251</v>
+      </c>
+      <c r="I23" t="s">
+        <v>260</v>
+      </c>
+      <c r="J23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" t="s">
+        <v>215</v>
+      </c>
+      <c r="E24" t="s">
+        <v>320</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" t="s">
+        <v>173</v>
+      </c>
+      <c r="H24" t="s">
+        <v>175</v>
+      </c>
+      <c r="I24" t="s">
         <v>174</v>
       </c>
-      <c r="D23" t="s">
-        <v>223</v>
-      </c>
-      <c r="E23" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" t="s">
-        <v>254</v>
-      </c>
-      <c r="G23" t="s">
-        <v>266</v>
-      </c>
-      <c r="H23" t="s">
-        <v>277</v>
-      </c>
-      <c r="I23" t="s">
-        <v>289</v>
+      <c r="J24" t="s">
+        <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>176</v>
-      </c>
-      <c r="B24" t="s">
-        <v>176</v>
-      </c>
-      <c r="C24" t="s">
-        <v>177</v>
-      </c>
-      <c r="D24" t="s">
-        <v>224</v>
-      </c>
-      <c r="E24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" t="s">
-        <v>178</v>
-      </c>
-      <c r="G24" t="s">
-        <v>180</v>
-      </c>
-      <c r="H24" t="s">
-        <v>179</v>
-      </c>
-      <c r="I24" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -4532,28 +4722,31 @@
         <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D25" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E25" t="s">
+        <v>321</v>
+      </c>
+      <c r="F25" t="s">
         <v>34</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>51</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>52</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>114</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -4561,86 +4754,95 @@
         <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D26" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E26" t="s">
+        <v>322</v>
+      </c>
+      <c r="F26" t="s">
         <v>34</v>
       </c>
-      <c r="F26" t="s">
-        <v>188</v>
-      </c>
       <c r="G26" t="s">
+        <v>183</v>
+      </c>
+      <c r="H26" t="s">
         <v>54</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>116</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C27" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D27" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E27" t="s">
+        <v>323</v>
+      </c>
+      <c r="F27" t="s">
         <v>34</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>55</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>56</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>118</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C28" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D28" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E28" t="s">
+        <v>324</v>
+      </c>
+      <c r="F28" t="s">
         <v>30</v>
       </c>
-      <c r="F28" t="s">
-        <v>190</v>
-      </c>
       <c r="G28" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="H28" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I28" t="s">
-        <v>193</v>
+        <v>186</v>
+      </c>
+      <c r="J28" t="s">
+        <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -4648,57 +4850,63 @@
         <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D29" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E29" t="s">
+        <v>325</v>
+      </c>
+      <c r="F29" t="s">
         <v>34</v>
       </c>
-      <c r="F29" t="s">
-        <v>194</v>
-      </c>
       <c r="G29" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H29" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I29" t="s">
-        <v>197</v>
+        <v>190</v>
+      </c>
+      <c r="J29" t="s">
+        <v>192</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C30" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D30" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="E30" t="s">
+        <v>326</v>
+      </c>
+      <c r="F30" t="s">
         <v>30</v>
       </c>
-      <c r="F30" t="s">
-        <v>198</v>
-      </c>
       <c r="G30" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="H30" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I30" t="s">
-        <v>311</v>
+        <v>194</v>
+      </c>
+      <c r="J30" t="s">
+        <v>291</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -4706,28 +4914,31 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D31" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="E31" t="s">
+        <v>327</v>
+      </c>
+      <c r="F31" t="s">
         <v>34</v>
       </c>
-      <c r="F31" t="s">
-        <v>233</v>
-      </c>
       <c r="G31" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="H31" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="I31" t="s">
-        <v>236</v>
+        <v>225</v>
+      </c>
+      <c r="J31" t="s">
+        <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -4735,33 +4946,37 @@
         <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D32" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="E32" t="s">
+        <v>328</v>
+      </c>
+      <c r="F32" t="s">
         <v>34</v>
       </c>
-      <c r="F32" t="s">
-        <v>237</v>
-      </c>
       <c r="G32" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="H32" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I32" t="s">
-        <v>240</v>
+        <v>229</v>
+      </c>
+      <c r="J32" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I32" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J32" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="A8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4772,7 +4987,7 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -4793,28 +5008,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" t="s">
         <v>134</v>
-      </c>
-      <c r="E1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -4822,7 +5037,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
@@ -4848,7 +5063,7 @@
         <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
@@ -4874,7 +5089,7 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -4892,7 +5107,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -4900,7 +5115,7 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="C5" t="s">
         <v>64</v>
@@ -4926,7 +5141,7 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
@@ -4944,7 +5159,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -4952,7 +5167,7 @@
         <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="C7" t="s">
         <v>64</v>
@@ -4970,7 +5185,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -4978,7 +5193,7 @@
         <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C8" t="s">
         <v>64</v>
@@ -5004,7 +5219,7 @@
         <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="C9" t="s">
         <v>64</v>
@@ -5056,7 +5271,7 @@
         <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="C11" t="s">
         <v>64</v>
@@ -5082,7 +5297,7 @@
         <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="C12" t="s">
         <v>64</v>
@@ -5108,7 +5323,7 @@
         <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="C13" t="s">
         <v>90</v>
@@ -5134,7 +5349,7 @@
         <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="C14" t="s">
         <v>90</v>
@@ -5160,7 +5375,7 @@
         <v>92</v>
       </c>
       <c r="B15" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="C15" t="s">
         <v>90</v>
@@ -5186,7 +5401,7 @@
         <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="C16" t="s">
         <v>90</v>
@@ -5204,7 +5419,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -5238,7 +5453,7 @@
         <v>98</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="C18" t="s">
         <v>90</v>

</xml_diff>